<commit_message>
Format annotated data, do simple evaluations
</commit_message>
<xml_diff>
--- a/Data/MarketIntelligenceReport_Annotation_Tasks.xlsx
+++ b/Data/MarketIntelligenceReport_Annotation_Tasks.xlsx
@@ -8,20 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\66 CausalMap\Panasonic-IDS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE40E69B-270C-4B1F-B23F-1F31B52A8390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10191545-8401-4D65-AE33-7B9F4636CACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-2964" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MarketIntelligenceReport_Task1" sheetId="1" r:id="rId1"/>
     <sheet name="MarketIntelligenceReport_Task2" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MarketIntelligenceReport_Task1!$A$1:$G$29</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId4"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="115">
   <si>
     <t>row_id</t>
   </si>
@@ -772,80 +779,6 @@
   </si>
   <si>
     <t>â€œcounter the use of faulty emission devices in engines, used in cars of a Japanese producer</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Prosecutors in Germany, Hungary, and Italy raided the offices of Suzuki this week over allegations that the automaker has been using a defeat device to fraudulently pass the jurisdictionâ€™s emissions tests.
-German officials said Wednesday that the investigation concerns people at Suzuki, whose European headquarters are in Germany, as well as Stellantis and parts supplier Marelli.
-The former supplied the Japanese automaker with diesel engines and the latter with parts for those engines, reports Reuters.
-The searches were conducted as part of a coordinated action by Eurojust, the European agency for criminal justice cooperation.
-This issue may have an impact on more than 22,000 vehicles, reports DW.
-Read Also: &lt;CAUSE&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Jeep And Suzuki Caught Cheating EUâ€™s Emission Rules With Grand Cherokee, Vitara, S-CrossThe searches were conducted &lt;/CAUSE&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in order to &lt;EFFECT&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">â€œcounter the use of faulty emission devices in engines, used in cars of a Japanese producer &lt;/EFFECT&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">,â€ Eurojust said.
-â€œ &lt;CAUSE&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The devices were allegedly fitted in the Italian-built diesel engines of large numbers of car</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>s &lt;/CAUSE&gt; , giving the impression that the vehiclesâ€™ nitrogen oxide emissions were in line with EU regulations.â€The engines were reportedly put in vehicles at Suzukiâ€™s production plant in Hungary that builds the SX4 S-Cross and the Vitara, which have been in production since 2013 and 2015, respectively.
-A Suzuki spokesperson told Reuters that the company was cooperating with European investigations.
-In Japan, Suzuki, along with Mazda and Yamaha, admitted to using false emission data for some vehicles in 2018.
-FCA, now a part of Stellantis, is in the process of resolving a U.S. fraud probe relating to diesel engines in Ram pickup trucks and Jeep vehicles</t>
-    </r>
   </si>
   <si>
     <t>The devices were allegedly fitted in the Italian-built diesel engines of large numbers of cars</t>
@@ -1456,60 +1389,6 @@
   </si>
   <si>
     <r>
-      <t>Tesla and India aren't ready for each other just yet.
-From to Uber and , many foreign companies have had to  launch low-price versions of their products  in a bid to  make inroads in the Indian market.
-It would be hard for Tesla to achieve mass-market volume in India necessary for a venture to make good business sense for the luxury car maker.
-Foreign or local electric cars (EVs) will grow in India only when there's price parity with its internal combustion engine (ICE) equivalent."
-"There is evidence suggesting that Tesla will succeed, but if not, Tesla will remain an automaker for the wealthy," he wrote.
-"&lt;CAUSE&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The key challenges to adoption of EVs in India are low penetration of charging infrastructure</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/CAUSE&gt;," said Mahesh Babu, CEO, Mahindra Electric, the electric vehicle division of Mahindra and Mahindra.
-"Given these conditions, it is understandable that&lt;EFFECT&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>local as well as foreign players may hesitate to expand in the Indian market</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/EFFECT&gt;."
-Mahindra Electric is leading the charge with its homegrown, battery-operated e2o Plus, a $10,000 car that goes about 87 miles per charge.
-We have the unique position of having years of experience of the Indian market as well as over 265 million kms (164 million miles) driven on our EVs.
-Mahesh Babu CEO, Mahindra Electric</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;EFFECT</t>
     </r>
     <r>
@@ -1563,12 +1442,81 @@
     </r>
   </si>
   <si>
+    <t>ce_lab</t>
+  </si>
+  <si>
     <t>pandemic</t>
   </si>
   <si>
     <t>invasion of Ukrain</t>
   </si>
   <si>
+    <t>customers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> to vote on mandatory CO2 standards for car manufacturers on Wednesday (11 May)</t>
+  </si>
+  <si>
+    <t>rising cost</t>
+  </si>
+  <si>
+    <t>road safety</t>
+  </si>
+  <si>
+    <t>automotive</t>
+  </si>
+  <si>
+    <t>Carbon Emission</t>
+  </si>
+  <si>
+    <t>unemployment</t>
+  </si>
+  <si>
+    <t>technology</t>
+  </si>
+  <si>
+    <t>sales</t>
+  </si>
+  <si>
+    <t>market expansion</t>
+  </si>
+  <si>
+    <t>demand and supply</t>
+  </si>
+  <si>
+    <t>charging infrastructure</t>
+  </si>
+  <si>
+    <t>investment</t>
+  </si>
+  <si>
+    <t>manufacturing and production</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tesla and India aren't ready for each other just yet.
+&lt;CAUSE&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>From to Uber and , many foreign companies have had to launch low-price versions of their products</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;/CAUSE&gt; in a bid to &lt;EFFECT&gt; </t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1577,7 +1525,252 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;EFFECT&gt; Russian vehicle sales plunged by 63 percent in March&lt;EFFECT&gt;</t>
+      <t>make inroads in the Indian market</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/EFFECT&gt;.
+It would be hard for Tesla to achieve mass-market volume in India necessary for a venture to make good business sense for the luxury car maker.
+Foreign or local electric cars (EVs) will grow in India only when there's price parity with its internal combustion engine (ICE) equivalent."
+"There is evidence suggesting that Tesla will succeed, but if not, Tesla will remain an automaker for the wealthy," he wrote.
+"The key challenges to adoption of EVs in India are low penetration of charging infrastructure," said Mahesh Babu, CEO, Mahindra Electric, the electric vehicle division of Mahindra and Mahindra.
+"Given these conditions, it is understandable that local as well as foreign players may hesitate to expand in the Indian market."
+Mahindra Electric is leading the charge with its homegrown, battery-operated e2o Plus, a $10,000 car that goes about 87 miles per charge.
+We have the unique position of having years of experience of the Indian market as well as over 265 million kms (164 million miles) driven on our EVs.
+Mahesh Babu CEO, Mahindra Electric</t>
+    </r>
+  </si>
+  <si>
+    <t>From to Uber and , many foreign companies have had to launch low-price versions of their products</t>
+  </si>
+  <si>
+    <t>matched</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>need to alter</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of matched</t>
+  </si>
+  <si>
+    <t>Additional</t>
+  </si>
+  <si>
+    <r>
+      <t>Tesla and India aren't ready for each other just yet.
+From to Uber and , many foreign companies have had to  launch low-price versions of their products  in a bid to  make inroads in the Indian market.
+It would be hard for Tesla to achieve mass-market volume in India necessary for a venture to make good business sense for the luxury car maker.
+Foreign or local electric cars (EVs) will grow in India only when there's price parity with its internal combustion engine (ICE) equivalent."
+"There is evidence suggesting that Tesla will succeed, but if not, Tesla will remain an automaker for the wealthy," he wrote.
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The key challenges to adoption of EVs in India are low penetration of charging infrastructure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">," said Mahesh Babu, CEO, Mahindra Electric, the electric vehicle division of Mahindra and Mahindra.
+"&lt;CAUSE&gt;Given these conditions&lt;/CAUSE&gt;, it is understandable that&lt;EFFECT&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>local as well as foreign players may hesitate to expand in the Indian market</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/EFFECT&gt;."
+Mahindra Electric is leading the charge with its homegrown, battery-operated e2o Plus, a $10,000 car that goes about 87 miles per charge.
+We have the unique position of having years of experience of the Indian market as well as over 265 million kms (164 million miles) driven on our EVs.
+Mahesh Babu CEO, Mahindra Electric</t>
+    </r>
+  </si>
+  <si>
+    <t>Given these conditions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The European Parliamentâ€™s environment committee (ENVI) is due </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to vote on mandatory CO2 standards for car manufacturers on Wednesday (11 May)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, with the possibility of calling for a 70% reduction target by 2030.
+Manufacturers are already being pushed to build cars that emit less CO2, including electric vehicles.
+&lt;CAUSE&gt;Wednesdayâ€™s vote will determine&lt;/CAUSE&gt;  &lt;EFFECT&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>how fast companies will have to transition production and when they will have to stop selling combustion engine vehicles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;/EFFECT&gt;.
+At the vote, MEPs are expected to propose a target of 70% reduction by 2030 in the number of vehicles being produced that emit greenhouse gases.
+By comparison, the European Commission has set a 55% reduction target for reducing CO2-emitting vehicles for 2030, and a full phase-out for 2050.
+A narrow majorityHowever, it may be difficult for the ENVI committee to adopt the ambitious 70% proposal.
+He added, â€œthis majority is narrow, 2 to 3 votes maximum, but it exists,â€ he added.
+Car manufacturer Stellantis, for example, has already announced that it will stop producing CO2-emitting cars by 2030 in the European market.
+German car manufacturer Volkswagen, for its part, said it aims to have electric vehicles account for 70% of its sales by the same date.
+After the vote in the ENVI committee, the European Parliament will vote in the plenary session in June</t>
+    </r>
+  </si>
+  <si>
+    <t>Wednesdayâ€™s vote will determine</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prosecutors in Germany, Hungary, and Italy raided the offices of Suzuki this week over allegations that the automaker has been using a defeat device to fraudulently pass the jurisdictionâ€™s emissions tests.
+German officials said Wednesday that the investigation concerns people at Suzuki, whose European headquarters are in Germany, as well as Stellantis and parts supplier Marelli.
+The former supplied the Japanese automaker with diesel engines and the latter with parts for those engines, reports Reuters.
+The searches were conducted as part of a coordinated action by Eurojust, the European agency for criminal justice cooperation.
+This issue may have an impact on more than 22,000 vehicles, reports DW.
+Read Also: &lt;CAUSE&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Jeep And Suzuki Caught Cheating EUâ€™s Emission Rules With Grand Cherokee, Vitara, S-CrossThe searches were conducted &lt;/CAUSE&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in order to &lt;EFFECT&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">â€œcounter the use of faulty emission devices in engines, used in cars of a Japanese producer &lt;/EFFECT&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,â€ Eurojust said.
+â€œ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The devices were allegedly fitted in the Italian-built diesel engines of large numbers of car</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s , giving the impression that the vehiclesâ€™ nitrogen oxide emissions were in line with EU regulations.â€The engines were reportedly put in vehicles at Suzukiâ€™s production plant in Hungary that builds the SX4 S-Cross and the Vitara, which have been in production since 2013 and 2015, respectively.
+A Suzuki spokesperson told Reuters that the company was cooperating with European investigations.
+In Japan, Suzuki, along with Mazda and Yamaha, admitted to using false emission data for some vehicles in 2018.
+FCA, now a part of Stellantis, is in the process of resolving a U.S. fraud probe relating to diesel engines in Ram pickup trucks and Jeep vehicles</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;EFFECT&gt; Russian vehicle sales plunged by 63 percent in March&lt;/EFFECT&gt;</t>
     </r>
     <r>
       <rPr>
@@ -1616,173 +1809,6 @@
 Renault at No.
 4 was down 65 percent and No.
 5 Toyota declined by 69 percent</t>
-    </r>
-  </si>
-  <si>
-    <t>customers</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> to vote on mandatory CO2 standards for car manufacturers on Wednesday (11 May)</t>
-  </si>
-  <si>
-    <r>
-      <t>The European Parliamentâ€™s environment committee (ENVI) is due &lt;CAUSE&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to vote on mandatory CO2 standards for car manufacturers on Wednesday (11 May) &lt;/CAUSE&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, with the possibility of calling for a 70% reduction target by 2030.
-Manufacturers are already being pushed to build cars that emit less CO2, including electric vehicles.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wednesdayâ€™s vote will determine &lt;EFFECT&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>how fast companies will have to transition production and when they will have to stop selling combustion engine vehicles</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;/EFFECT&gt;.
-At the vote, MEPs are expected to propose a target of 70% reduction by 2030 in the number of vehicles being produced that emit greenhouse gases.
-By comparison, the European Commission has set a 55% reduction target for reducing CO2-emitting vehicles for 2030, and a full phase-out for 2050.
-A narrow majorityHowever, it may be difficult for the ENVI committee to adopt the ambitious 70% proposal.
-He added, â€œthis majority is narrow, 2 to 3 votes maximum, but it exists,â€ he added.
-Car manufacturer Stellantis, for example, has already announced that it will stop producing CO2-emitting cars by 2030 in the European market.
-German car manufacturer Volkswagen, for its part, said it aims to have electric vehicles account for 70% of its sales by the same date.
-After the vote in the ENVI committee, the European Parliament will vote in the plenary session in June</t>
-    </r>
-  </si>
-  <si>
-    <t>rising cost</t>
-  </si>
-  <si>
-    <t>road safety</t>
-  </si>
-  <si>
-    <t>automotive</t>
-  </si>
-  <si>
-    <t>Carbon Emission</t>
-  </si>
-  <si>
-    <t>unemployment</t>
-  </si>
-  <si>
-    <t>technology</t>
-  </si>
-  <si>
-    <t>sales</t>
-  </si>
-  <si>
-    <t>market expansion</t>
-  </si>
-  <si>
-    <t>demand and supply</t>
-  </si>
-  <si>
-    <t>charging infrastructure</t>
-  </si>
-  <si>
-    <t>investment</t>
-  </si>
-  <si>
-    <t>manufacturing and production</t>
-  </si>
-  <si>
-    <t>From to Uber and , many foreign companies have had to launch low-price versions of their products</t>
-  </si>
-  <si>
-    <t>ce_label</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;CAUSE&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>From to Uber and , many foreign companies have had to launch low-price versions of their products</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;/CAUSE&gt; in a bid to &lt;EFFECT&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>make inroads in the Indian market</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/EFFECT&gt;.</t>
     </r>
   </si>
 </sst>
@@ -1940,7 +1966,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2126,6 +2152,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -2287,25 +2319,25 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2363,6 +2395,165 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Fiona Tan" refreshedDate="44995.503173611112" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="29" xr:uid="{43BF5F72-659C-4C1F-9DE8-515B2128B48A}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="F1:F1048576" sheet="MarketIntelligenceReport_Task1"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="matched" numFmtId="0">
+      <sharedItems containsBlank="1" count="3">
+        <s v="No"/>
+        <s v="Yes"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="29">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D369ACD3-2D93-4DCB-90B9-D74793477FF1}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item h="1" x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of matched" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2664,339 +2855,383 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="1"/>
-    <col min="3" max="3" width="66.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="7.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="3"/>
+    <col min="3" max="3" width="171" style="3" customWidth="1"/>
+    <col min="4" max="5" width="14.5546875" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="210" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>51</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>52</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1">
+    </row>
+    <row r="3" spans="1:7" ht="179.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>51</v>
       </c>
-      <c r="G2" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>51</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>52</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="F3" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="288.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>78</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>79</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="F4" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>78</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>79</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="F5" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="145.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>235</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>236</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="F6" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>235</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>236</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="F7" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="145.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>235</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>236</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="F8" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="273" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>292</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>293</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="F9" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>373</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <v>374</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="F10" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>373</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="1">
         <v>374</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="F11" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>456</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="1">
         <v>457</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="C12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="F12" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="294.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>551</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="1">
         <v>552</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="F13" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="222.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>682</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="1">
         <v>683</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="F14" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>682</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="1">
         <v>683</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="F15" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>682</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="1">
         <v>683</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="F16" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>682</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="1">
         <v>683</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="F17" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="200.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>786</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="1">
         <v>102</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="232.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>949</v>
       </c>
@@ -3004,7 +3239,7 @@
         <v>273</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>50</v>
@@ -3012,8 +3247,11 @@
       <c r="E19" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="232.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>949</v>
       </c>
@@ -3021,16 +3259,19 @@
         <v>273</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="213.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>1117</v>
       </c>
@@ -3038,16 +3279,19 @@
         <v>442</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="213.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>1117</v>
       </c>
@@ -3055,16 +3299,19 @@
         <v>442</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="321" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>2397</v>
       </c>
@@ -3072,16 +3319,19 @@
         <v>388</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="321" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>2397</v>
       </c>
@@ -3089,16 +3339,19 @@
         <v>388</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="299.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>2397</v>
       </c>
@@ -3106,16 +3359,19 @@
         <v>388</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="223.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>2865</v>
       </c>
@@ -3123,16 +3379,19 @@
         <v>70</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="228.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>4256</v>
       </c>
@@ -3140,16 +3399,19 @@
         <v>134</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="275.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>7831</v>
       </c>
@@ -3157,16 +3419,19 @@
         <v>32</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>7831</v>
       </c>
@@ -3174,16 +3439,20 @@
         <v>32</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>81</v>
+      <c r="F29" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G29" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3194,990 +3463,1049 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="2"/>
-    <col min="5" max="5" width="29.44140625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="137" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="3"/>
+    <col min="5" max="5" width="29.44140625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>51</v>
+      </c>
+      <c r="D2" s="1">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>51</v>
+      </c>
+      <c r="D3" s="1">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>78</v>
+      </c>
+      <c r="D4" s="1">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>78</v>
+      </c>
+      <c r="D5" s="1">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>235</v>
+      </c>
+      <c r="D6" s="1">
+        <v>236</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>235</v>
+      </c>
+      <c r="D7" s="1">
+        <v>236</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>235</v>
+      </c>
+      <c r="D8" s="1">
+        <v>236</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>292</v>
+      </c>
+      <c r="D9" s="1">
+        <v>293</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>373</v>
+      </c>
+      <c r="D10" s="1">
+        <v>374</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>373</v>
+      </c>
+      <c r="D11" s="1">
+        <v>374</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>456</v>
+      </c>
+      <c r="D12" s="1">
+        <v>457</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>551</v>
+      </c>
+      <c r="D13" s="1">
+        <v>552</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>682</v>
+      </c>
+      <c r="D14" s="1">
+        <v>683</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>682</v>
+      </c>
+      <c r="D15" s="1">
+        <v>683</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>682</v>
+      </c>
+      <c r="D16" s="1">
+        <v>683</v>
+      </c>
+      <c r="E16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>682</v>
+      </c>
+      <c r="D17" s="1">
+        <v>683</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>786</v>
+      </c>
+      <c r="D18" s="1">
         <v>102</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C19" s="1">
+        <v>949</v>
+      </c>
+      <c r="D19" s="1">
+        <v>273</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>949</v>
+      </c>
+      <c r="D20" s="1">
+        <v>273</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1117</v>
+      </c>
+      <c r="D21" s="1">
+        <v>442</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1117</v>
+      </c>
+      <c r="D22" s="1">
+        <v>442</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2397</v>
+      </c>
+      <c r="D23" s="1">
+        <v>388</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2397</v>
+      </c>
+      <c r="D24" s="1">
+        <v>388</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2397</v>
+      </c>
+      <c r="D25" s="1">
+        <v>388</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2865</v>
+      </c>
+      <c r="D26" s="1">
+        <v>70</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4256</v>
+      </c>
+      <c r="D27" s="1">
+        <v>134</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1">
+        <v>7831</v>
+      </c>
+      <c r="D28" s="1">
+        <v>32</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1">
+        <v>7831</v>
+      </c>
+      <c r="D29" s="1">
+        <v>32</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1">
         <v>51</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D30" s="1">
         <v>52</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="E30" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1">
         <v>51</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D31" s="1">
         <v>52</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="E31" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1">
         <v>78</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D32" s="1">
         <v>79</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="E32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1">
         <v>78</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D33" s="1">
         <v>79</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="E33" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1">
         <v>235</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D34" s="1">
         <v>236</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="E34" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1">
         <v>235</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D35" s="1">
         <v>236</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="E35" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1">
         <v>235</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D36" s="1">
         <v>236</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="E36" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1">
         <v>292</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D37" s="1">
         <v>293</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="E37" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1">
         <v>373</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D38" s="1">
         <v>374</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="E38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="1">
         <v>373</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D39" s="1">
         <v>374</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="E39" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1">
+        <v>456</v>
+      </c>
+      <c r="D40" s="1">
+        <v>457</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1">
+        <v>551</v>
+      </c>
+      <c r="D41" s="1">
+        <v>552</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1">
+        <v>682</v>
+      </c>
+      <c r="D42" s="1">
+        <v>683</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2">
-        <v>456</v>
-      </c>
-      <c r="D12" s="2">
-        <v>457</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2">
-        <v>551</v>
-      </c>
-      <c r="D13" s="2">
-        <v>552</v>
-      </c>
-      <c r="E13" s="2" t="s">
+    </row>
+    <row r="43" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="1">
+        <v>682</v>
+      </c>
+      <c r="D43" s="1">
+        <v>683</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="1">
+        <v>682</v>
+      </c>
+      <c r="D44" s="1">
+        <v>683</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2">
+    <row r="45" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1">
         <v>682</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D45" s="1">
         <v>683</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="2">
-        <v>682</v>
-      </c>
-      <c r="D15" s="2">
-        <v>683</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2">
-        <v>682</v>
-      </c>
-      <c r="D16" s="2">
-        <v>683</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2">
-        <v>682</v>
-      </c>
-      <c r="D17" s="2">
-        <v>683</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="E45" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="1">
         <v>786</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D46" s="1">
         <v>102</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="E46" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1">
         <v>949</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D47" s="1">
         <v>273</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="E47" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="1">
         <v>949</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D48" s="1">
         <v>273</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="E48" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="1">
         <v>1117</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D49" s="1">
         <v>442</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="E49" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
         <v>1117</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D50" s="1">
         <v>442</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E50" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="2">
+    <row r="51" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1">
         <v>2397</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D51" s="1">
         <v>388</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E51" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2397</v>
+      </c>
+      <c r="D52" s="1">
+        <v>388</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="2">
+    <row r="53" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="1">
         <v>2397</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D53" s="1">
         <v>388</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="2">
-        <v>2397</v>
-      </c>
-      <c r="D25" s="2">
-        <v>388</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="E53" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="B54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1">
         <v>2865</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D54" s="1">
         <v>70</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="E54" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="2">
+      <c r="B55" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="1">
         <v>4256</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D55" s="1">
         <v>134</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="E55" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="1">
         <v>7831</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D56" s="1">
         <v>32</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="E56" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="1">
         <v>7831</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D57" s="1">
         <v>32</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="2">
-        <v>51</v>
-      </c>
-      <c r="D30" s="2">
-        <v>52</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="2">
-        <v>51</v>
-      </c>
-      <c r="D31" s="2">
-        <v>52</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="2">
-        <v>78</v>
-      </c>
-      <c r="D32" s="2">
-        <v>79</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2">
-        <v>78</v>
-      </c>
-      <c r="D33" s="2">
-        <v>79</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2">
-        <v>235</v>
-      </c>
-      <c r="D34" s="2">
-        <v>236</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="2">
-        <v>235</v>
-      </c>
-      <c r="D35" s="2">
-        <v>236</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="2">
-        <v>235</v>
-      </c>
-      <c r="D36" s="2">
-        <v>236</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="2">
-        <v>292</v>
-      </c>
-      <c r="D37" s="2">
-        <v>293</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="2">
-        <v>373</v>
-      </c>
-      <c r="D38" s="2">
-        <v>374</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="2">
-        <v>373</v>
-      </c>
-      <c r="D39" s="2">
-        <v>374</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="2">
-        <v>456</v>
-      </c>
-      <c r="D40" s="2">
-        <v>457</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="2">
-        <v>551</v>
-      </c>
-      <c r="D41" s="2">
-        <v>552</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="2">
-        <v>682</v>
-      </c>
-      <c r="D42" s="2">
-        <v>683</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="2">
-        <v>682</v>
-      </c>
-      <c r="D43" s="2">
-        <v>683</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="2">
-        <v>682</v>
-      </c>
-      <c r="D44" s="2">
-        <v>683</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="2">
-        <v>682</v>
-      </c>
-      <c r="D45" s="2">
-        <v>683</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="2">
-        <v>786</v>
-      </c>
-      <c r="D46" s="2">
-        <v>102</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="2">
-        <v>949</v>
-      </c>
-      <c r="D47" s="2">
-        <v>273</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="2">
-        <v>949</v>
-      </c>
-      <c r="D48" s="2">
-        <v>273</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" s="2">
-        <v>1117</v>
-      </c>
-      <c r="D49" s="2">
-        <v>442</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="2">
-        <v>1117</v>
-      </c>
-      <c r="D50" s="2">
-        <v>442</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="2">
-        <v>2397</v>
-      </c>
-      <c r="D51" s="2">
-        <v>388</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="2">
-        <v>2397</v>
-      </c>
-      <c r="D52" s="2">
-        <v>388</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="2">
-        <v>2397</v>
-      </c>
-      <c r="D53" s="2">
-        <v>388</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" s="2">
-        <v>2865</v>
-      </c>
-      <c r="D54" s="2">
-        <v>70</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55" s="2">
-        <v>4256</v>
-      </c>
-      <c r="D55" s="2">
-        <v>134</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C56" s="2">
-        <v>7831</v>
-      </c>
-      <c r="D56" s="2">
-        <v>32</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="2">
-        <v>7831</v>
-      </c>
-      <c r="D57" s="2">
-        <v>32</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>84</v>
+      <c r="E57" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE50FF9-E6D4-4D78-8CC1-E44FB0D89FC6}">
+  <dimension ref="A3:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="7">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update data and codes up to point of paper submission
</commit_message>
<xml_diff>
--- a/Data/MarketIntelligenceReport_Annotation_Tasks.xlsx
+++ b/Data/MarketIntelligenceReport_Annotation_Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\66 CausalMap\Panasonic-IDS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5332EC32-E475-40C6-8858-588E630568DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334C4245-E6E9-4087-A1E5-7477ACB87BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-2964" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,17 @@
     <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MarketIntelligenceReport_Task1!$A$1:$G$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MarketIntelligenceReport_Task1!$A$1:$G$30</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId4"/>
+    <pivotCache cacheId="21" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="118">
   <si>
     <t>row_id</t>
   </si>
@@ -127,60 +127,6 @@
   </si>
   <si>
     <t>topic</t>
-  </si>
-  <si>
-    <r>
-      <t>FILE PHOTO: The 2018 Camry XSE is introduced during the North American International Auto Show in Detroit, Michigan, U.S., January 9, 2017.
-The reportâ€™s focus solely on electric vehicles marks a shift away from the current policy that incentivises both hybrid vehicles - which combine fossil fuel and electric power - and electric cars, and is worrying some automakers.
-Indiaâ€™s plan to leapfrog hybrid technology comes after China announced aggressive measures last year to push sales of plug-in vehicles including subsidies, research funding and rules designed to discourage fossil-fuel cars in big cities.
-Mahindra &amp; Mahindra is the only manufacturer of electric vehicles in India.
-The new Niti Aayog report, co-produced with U.S. consultancy Rocky Mountain Institute, outlines a 15-year plan, broken into three phases starting in 2017.
-â€œLimit registration of conventional vehicles through public lotteries and complement that with preferential registration for electric vehicles, similar to that in China,â€ the report said, in one of its most radical proposals.
-To kick-start the shift, the report suggests &lt;CAUSE&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> bulk procurement of electric vehicles, building standardized, swappable batteries for two- and three-wheelers </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/CAUSE&gt; to &lt;EFFECT&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bring down their cost and having favorable tariff structures for charging cars</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;/EFFECT&gt;.
-It also recommends setting up battery swapping stations by 2018, common manufacturing facilities for components and increasing subsidies on all battery electric vehicles to bring them to cost parity with conventional models by 2025.
-Other suggestions in the blueprint include incentivising the use of electric cars as taxis by lowering taxes, interest rates on loans for purchases and electricity tariffs for fleet operators, and lowering duties on makers of such fleet cars.
-â€œAll cars being electric is a distant dream.â€</t>
-    </r>
   </si>
   <si>
     <r>
@@ -499,59 +445,6 @@
   <si>
     <r>
       <t xml:space="preserve">Union minister Nitin Gadkari on Tuesday in New Delhi said that efforts are being made to improve road engineering, automobile manufacturing, and emergency services, and the cooperation of all stakeholders is necessary to improve road safety.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;CAUSE&gt; The government is also planning to conduct a road safety audit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;/CAUSE&gt; to</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;EFFECT&gt; improve the quality of roads and reduce accidents &lt;/EFFECT&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, the minister of road transport and highways said.
-Speaking to the reporters on the sidelines of the AIMA National Management Convention, the minister also termed the death of former Tata Sons chairman Cyrus Mistry earlier this month as "very unfortunate" and shocking.
-On road safety, he said, the education and cooperation of people are very important and various initiatives through campaigns and advertisements are being taken to improve the safety of people on the road.
-"....road safety is the highest agenda for all of us," Gadkari said.
-The minister also said that on September 28 he will kick off a trial project involving Toyota's new car that will be powered by flex-fuel.
-"That day is not far when the cars will run 100 per cent on ethanol instead of petrol," the minister said, adding that as a result pollution will be reduced, import bill will come down, and ultimately the farmers will be benefitted.
-Mistry, 54, was killed in a car crash in Maharashtra's Palghar district near Mumbai on September 4 when his luxury car hit a road divider.
-Mistry, an Irish citizen, and scion of the real estate behemoth Shapoorji Pallonji Group were travelling from Ahmedabad to Mumbai</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Union minister Nitin Gadkari on Tuesday in New Delhi said that efforts are being made to improve road engineering, automobile manufacturing, and emergency services, and the cooperation of all stakeholders is necessary to improve road safety.
 The government is also planning to conduct a road safety audit to improve the quality of roads and reduce accidents, the minister of road transport and highways said.
 Speaking to the reporters on the sidelines of the AIMA National Management Convention, the minister also termed the death of former Tata Sons chairman Cyrus Mistry earlier this month as "very unfortunate" and shocking.
 On road safety, he said, &lt;CAUSE&gt; </t>
@@ -716,60 +609,6 @@
   </si>
   <si>
     <t xml:space="preserve"> increase the production of the future-generation electrified dual-clutch transmissions (eDCT) (pictured, below) for Stellantis hybrid and PHEVs</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Stellantis announces two major initiatives in Italy in a bid to boost its electric powertrain offering and reduce its carbon footprint.
-&lt;CAUSE&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>To advance its electrified model range, the automaker has signed a new agreement with Punch Powertrain &lt;/CAUSE&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;EFFECT&gt; increase the production of the future-generation electrified dual-clutch transmissions (eDCT) (pictured, below) for Stellantis hybrid and PHEVs  &lt;/EFFECT&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> .
-The upgraded facility, developed within the Mirafiori Complex in Turin, Italy, will complement existing capacity in Metz, France.
-Stellantis also announces the Mirafiori Complex will be home to its Circular Economy Hub, starting with three activities for the sustainable use of vehicles and parts.
-These include vehicle reconditioning, vehicle dismantling and parts remanufacturing, with the scope set to expand further globally.
-The ambition for its Circular Economy Business Unit is to quadruple extended life revenues for parts and services and multiply recycling revenues tenfold by 2030 as compared to 2021.
-This district serves as a vehicle production hub, an electrification engineering center and the heart of design for iconic Italian brands.
-Investment also will be seen at the Melfi facility, together with Sochaux in France, host to the new electric platform called STLA Medium.
-The platform is specifically designed for the battery-electric vehicle market, claims a high level of flexibility and is expected to achieve a range up to 440 miles (708 km).
-Stellantis has invested more than â‚¬5 billion ($4.9 billion) in the past four years in Italian operations for new products and manufacturing sites</t>
-    </r>
   </si>
   <si>
     <t>To advance its electrified model range, the automaker has signed a new agreement with Punch Powertrain</t>
@@ -1571,80 +1410,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Prosecutors in Germany, Hungary, and Italy raided the offices of Suzuki this week over allegations that the automaker has been using a defeat device to fraudulently pass the jurisdictionâ€™s emissions tests.
-German officials said Wednesday that the investigation concerns people at Suzuki, whose European headquarters are in Germany, as well as Stellantis and parts supplier Marelli.
-The former supplied the Japanese automaker with diesel engines and the latter with parts for those engines, reports Reuters.
-The searches were conducted as part of a coordinated action by Eurojust, the European agency for criminal justice cooperation.
-This issue may have an impact on more than 22,000 vehicles, reports DW.
-Read Also: &lt;CAUSE&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Jeep And Suzuki Caught Cheating EUâ€™s Emission Rules With Grand Cherokee, Vitara, S-CrossThe searches were conducted &lt;/CAUSE&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in order to &lt;EFFECT&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">â€œcounter the use of faulty emission devices in engines, used in cars of a Japanese producer &lt;/EFFECT&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">,â€ Eurojust said.
-â€œ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The devices were allegedly fitted in the Italian-built diesel engines of large numbers of car</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>s , giving the impression that the vehiclesâ€™ nitrogen oxide emissions were in line with EU regulations.â€The engines were reportedly put in vehicles at Suzukiâ€™s production plant in Hungary that builds the SX4 S-Cross and the Vitara, which have been in production since 2013 and 2015, respectively.
-A Suzuki spokesperson told Reuters that the company was cooperating with European investigations.
-In Japan, Suzuki, along with Mazda and Yamaha, admitted to using false emission data for some vehicles in 2018.
-FCA, now a part of Stellantis, is in the process of resolving a U.S. fraud probe relating to diesel engines in Ram pickup trucks and Jeep vehicles</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="11"/>
         <color theme="4"/>
@@ -1806,6 +1571,295 @@
   </si>
   <si>
     <t>to make inroads in the Indian market</t>
+  </si>
+  <si>
+    <r>
+      <t>FILE PHOTO: The 2018 Camry XSE is introduced during the North American International Auto Show in Detroit, Michigan, U.S., January 9, 2017.
+The reportâ€™s focus solely on electric vehicles marks a shift away from the current policy that incentivises both hybrid vehicles - which combine fossil fuel and electric power - and electric cars, and is worrying some automakers.
+Indiaâ€™s plan to leapfrog hybrid technology comes after China announced aggressive measures last year to push sales of plug-in vehicles including subsidies, research funding and rules designed to discourage fossil-fuel cars in big cities.
+Mahindra &amp; Mahindra is the only manufacturer of electric vehicles in India.
+The new Niti Aayog report, co-produced with U.S. consultancy Rocky Mountain Institute, outlines a 15-year plan, broken into three phases starting in 2017.
+â€œLimit registration of conventional vehicles through public lotteries and complement that with preferential registration for electric vehicles, similar to that in China,â€ the report said, in one of its most radical proposals.
+To kick-start the shift, the report suggests &lt;EFFECT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bulk procurement of electric vehicles, building standardized, swappable batteries for two- and three-wheelers </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/EFFECT&gt; &lt;CAUSE&gt;to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bring down their cost and having favorable tariff structures for charging cars</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/CAUSE&gt;.
+It also recommends setting up battery swapping stations by 2018, common manufacturing facilities for components and increasing subsidies on all battery electric vehicles to bring them to cost parity with conventional models by 2025.
+Other suggestions in the blueprint include incentivising the use of electric cars as taxis by lowering taxes, interest rates on loans for purchases and electricity tariffs for fleet operators, and lowering duties on makers of such fleet cars.
+â€œAll cars being electric is a distant dream.â€</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Stellantis announces two major initiatives in Italy in a bid to boost its electric powertrain offering and reduce its carbon footprint.
+&lt;EFFECT&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To advance its electrified model range, the automaker has signed a new agreement with Punch Powertrain &lt;/EFFECT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;CAUSE&gt;to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> increase the production of the future-generation electrified dual-clutch transmissions (eDCT) (pictured, below) for Stellantis hybrid and PHEVs  &lt;/CAUSE&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> .
+The upgraded facility, developed within the Mirafiori Complex in Turin, Italy, will complement existing capacity in Metz, France.
+Stellantis also announces the Mirafiori Complex will be home to its Circular Economy Hub, starting with three activities for the sustainable use of vehicles and parts.
+These include vehicle reconditioning, vehicle dismantling and parts remanufacturing, with the scope set to expand further globally.
+The ambition for its Circular Economy Business Unit is to quadruple extended life revenues for parts and services and multiply recycling revenues tenfold by 2030 as compared to 2021.
+This district serves as a vehicle production hub, an electrification engineering center and the heart of design for iconic Italian brands.
+Investment also will be seen at the Melfi facility, together with Sochaux in France, host to the new electric platform called STLA Medium.
+The platform is specifically designed for the battery-electric vehicle market, claims a high level of flexibility and is expected to achieve a range up to 440 miles (708 km).
+Stellantis has invested more than â‚¬5 billion ($4.9 billion) in the past four years in Italian operations for new products and manufacturing sites</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Stellantis announces two major initiatives in Italy in a bid to boost its electric powertrain offering and reduce its carbon footprint.
+&lt;CAUSE&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To advance its electrified model range &lt;/CAUSE&gt;, &lt;EFFECT&gt;the automaker has signed a new agreement with Punch Powertrain &lt;/EFFECT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> increase the production of the future-generation electrified dual-clutch transmissions (eDCT) (pictured, below) for Stellantis hybrid and PHEVs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> .
+The upgraded facility, developed within the Mirafiori Complex in Turin, Italy, will complement existing capacity in Metz, France.
+Stellantis also announces the Mirafiori Complex will be home to its Circular Economy Hub, starting with three activities for the sustainable use of vehicles and parts.
+These include vehicle reconditioning, vehicle dismantling and parts remanufacturing, with the scope set to expand further globally.
+The ambition for its Circular Economy Business Unit is to quadruple extended life revenues for parts and services and multiply recycling revenues tenfold by 2030 as compared to 2021.
+This district serves as a vehicle production hub, an electrification engineering center and the heart of design for iconic Italian brands.
+Investment also will be seen at the Melfi facility, together with Sochaux in France, host to the new electric platform called STLA Medium.
+The platform is specifically designed for the battery-electric vehicle market, claims a high level of flexibility and is expected to achieve a range up to 440 miles (708 km).
+Stellantis has invested more than â‚¬5 billion ($4.9 billion) in the past four years in Italian operations for new products and manufacturing sites</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prosecutors in Germany, Hungary, and Italy raided the offices of Suzuki this week over allegations that the automaker has been using a defeat device to fraudulently pass the jurisdictionâ€™s emissions tests.
+German officials said Wednesday that the investigation concerns people at Suzuki, whose European headquarters are in Germany, as well as Stellantis and parts supplier Marelli.
+The former supplied the Japanese automaker with diesel engines and the latter with parts for those engines, reports Reuters.
+The searches were conducted as part of a coordinated action by Eurojust, the European agency for criminal justice cooperation.
+This issue may have an impact on more than 22,000 vehicles, reports DW.
+Read Also: &lt;EFFECT&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Jeep And Suzuki Caught Cheating EUâ€™s Emission Rules With Grand Cherokee, Vitara, S-CrossThe searches were conducted &lt;/EFFECT&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in order &lt;CAUSE&gt;to “counter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the use of faulty emission devices in engines, used in cars of a Japanese producer &lt;/CAUSE&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,â€ Eurojust said.
+â€œ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The devices were allegedly fitted in the Italian-built diesel engines of large numbers of car</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s , giving the impression that the vehiclesâ€™ nitrogen oxide emissions were in line with EU regulations.â€The engines were reportedly put in vehicles at Suzukiâ€™s production plant in Hungary that builds the SX4 S-Cross and the Vitara, which have been in production since 2013 and 2015, respectively.
+A Suzuki spokesperson told Reuters that the company was cooperating with European investigations.
+In Japan, Suzuki, along with Mazda and Yamaha, admitted to using false emission data for some vehicles in 2018.
+FCA, now a part of Stellantis, is in the process of resolving a U.S. fraud probe relating to diesel engines in Ram pickup trucks and Jeep vehicles</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Union minister Nitin Gadkari on Tuesday in New Delhi said that efforts are being made to improve road engineering, automobile manufacturing, and emergency services, and the cooperation of all stakeholders is necessary to improve road safety.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;EFFECT&gt; The government is also planning to conduct a road safety audit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/EFFECT&gt; &lt;CAUSE&gt;to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> improve the quality of roads and reduce accidents &lt;/CAUSE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, the minister of road transport and highways said.
+Speaking to the reporters on the sidelines of the AIMA National Management Convention, the minister also termed the death of former Tata Sons chairman Cyrus Mistry earlier this month as "very unfortunate" and shocking.
+On road safety, he said, the education and cooperation of people are very important and various initiatives through campaigns and advertisements are being taken to improve the safety of people on the road.
+"....road safety is the highest agenda for all of us," Gadkari said.
+The minister also said that on September 28 he will kick off a trial project involving Toyota's new car that will be powered by flex-fuel.
+"That day is not far when the cars will run 100 per cent on ethanol instead of petrol," the minister said, adding that as a result pollution will be reduced, import bill will come down, and ultimately the farmers will be benefitted.
+Mistry, 54, was killed in a car crash in Maharashtra's Palghar district near Mumbai on September 4 when his luxury car hit a road divider.
+Mistry, an Irish citizen, and scion of the real estate behemoth Shapoorji Pallonji Group were travelling from Ahmedabad to Mumbai</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2519,7 +2573,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D369ACD3-2D93-4DCB-90B9-D74793477FF1}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D369ACD3-2D93-4DCB-90B9-D74793477FF1}" name="PivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -2860,10 +2914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2892,10 +2946,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="210" customHeight="1" x14ac:dyDescent="0.3">
@@ -2906,16 +2960,16 @@
         <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="179.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2926,16 +2980,16 @@
         <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="288.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2946,7 +3000,7 @@
         <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -2955,7 +3009,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
@@ -2966,7 +3020,7 @@
         <v>79</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>30</v>
@@ -2975,7 +3029,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="145.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2986,7 +3040,7 @@
         <v>236</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -2995,7 +3049,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="135" customHeight="1" x14ac:dyDescent="0.3">
@@ -3006,7 +3060,7 @@
         <v>236</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -3015,7 +3069,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="145.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3026,7 +3080,7 @@
         <v>236</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
@@ -3035,7 +3089,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="273" customHeight="1" x14ac:dyDescent="0.3">
@@ -3045,8 +3099,8 @@
       <c r="B9" s="1">
         <v>293</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
+      <c r="C9" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
@@ -3055,7 +3109,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3066,7 +3120,7 @@
         <v>374</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>19</v>
@@ -3075,7 +3129,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="144" x14ac:dyDescent="0.3">
@@ -3086,7 +3140,7 @@
         <v>374</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>20</v>
@@ -3095,7 +3149,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="192" customHeight="1" x14ac:dyDescent="0.3">
@@ -3106,16 +3160,16 @@
         <v>457</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="294.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3126,7 +3180,7 @@
         <v>552</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>23</v>
@@ -3135,7 +3189,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="222.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3145,17 +3199,17 @@
       <c r="B14" s="1">
         <v>683</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
+      <c r="C14" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
@@ -3166,7 +3220,7 @@
         <v>683</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>26</v>
@@ -3175,7 +3229,7 @@
         <v>27</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
@@ -3186,16 +3240,16 @@
         <v>683</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
@@ -3206,7 +3260,7 @@
         <v>683</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>28</v>
@@ -3215,7 +3269,7 @@
         <v>29</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="200.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3225,37 +3279,37 @@
       <c r="B18" s="1">
         <v>102</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>48</v>
+      <c r="C18" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="232.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>949</v>
-      </c>
-      <c r="B19" s="3">
-        <v>273</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>51</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="200.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>786</v>
+      </c>
+      <c r="B19" s="1">
+        <v>102</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="232.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3265,37 +3319,37 @@
       <c r="B20" s="3">
         <v>273</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>53</v>
+      <c r="C20" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="213.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="232.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>1117</v>
+        <v>949</v>
       </c>
       <c r="B21" s="3">
-        <v>442</v>
+        <v>273</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="213.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3306,36 +3360,36 @@
         <v>442</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="321" customHeight="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="213.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>2397</v>
+        <v>1117</v>
       </c>
       <c r="B23" s="3">
-        <v>388</v>
+        <v>442</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="321" customHeight="1" x14ac:dyDescent="0.3">
@@ -3346,19 +3400,19 @@
         <v>388</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="299.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="321" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>2397</v>
       </c>
@@ -3366,79 +3420,79 @@
         <v>388</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="299.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>2397</v>
+      </c>
+      <c r="B26" s="3">
+        <v>388</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="223.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>2865</v>
+      </c>
+      <c r="B27" s="3">
+        <v>70</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="223.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
-        <v>2865</v>
-      </c>
-      <c r="B26" s="3">
+      <c r="F27" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="228.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>4256</v>
+      </c>
+      <c r="B28" s="3">
+        <v>134</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="228.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
-        <v>4256</v>
-      </c>
-      <c r="B27" s="3">
-        <v>134</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="275.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
-        <v>7831</v>
-      </c>
-      <c r="B28" s="3">
-        <v>32</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="F28" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="275.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>7831</v>
       </c>
@@ -3446,20 +3500,40 @@
         <v>32</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>7831</v>
+      </c>
+      <c r="B30" s="3">
+        <v>32</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G29" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G30" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3488,7 +3562,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -3502,7 +3576,7 @@
     </row>
     <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -3514,7 +3588,7 @@
         <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3531,7 +3605,7 @@
         <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3548,7 +3622,7 @@
         <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3565,7 +3639,7 @@
         <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3582,7 +3656,7 @@
         <v>236</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3599,7 +3673,7 @@
         <v>236</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3616,7 +3690,7 @@
         <v>236</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3633,7 +3707,7 @@
         <v>293</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3650,7 +3724,7 @@
         <v>374</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3667,12 +3741,12 @@
         <v>374</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -3684,7 +3758,7 @@
         <v>457</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3701,12 +3775,12 @@
         <v>552</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -3718,7 +3792,7 @@
         <v>683</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3735,12 +3809,12 @@
         <v>683</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -3752,7 +3826,7 @@
         <v>683</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3769,12 +3843,12 @@
         <v>683</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>3</v>
@@ -3786,12 +3860,12 @@
         <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -3803,12 +3877,12 @@
         <v>273</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>3</v>
@@ -3820,12 +3894,12 @@
         <v>273</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>3</v>
@@ -3837,12 +3911,12 @@
         <v>442</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>3</v>
@@ -3854,12 +3928,12 @@
         <v>442</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>3</v>
@@ -3871,12 +3945,12 @@
         <v>388</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>3</v>
@@ -3888,12 +3962,12 @@
         <v>388</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
@@ -3905,12 +3979,12 @@
         <v>388</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>3</v>
@@ -3922,12 +3996,12 @@
         <v>70</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
@@ -3939,12 +4013,12 @@
         <v>134</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>3</v>
@@ -3956,12 +4030,12 @@
         <v>32</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
@@ -3973,7 +4047,7 @@
         <v>32</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3990,7 +4064,7 @@
         <v>52</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4007,7 +4081,7 @@
         <v>52</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4024,7 +4098,7 @@
         <v>79</v>
       </c>
       <c r="E32" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4041,7 +4115,7 @@
         <v>79</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4058,7 +4132,7 @@
         <v>236</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4075,7 +4149,7 @@
         <v>236</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4092,7 +4166,7 @@
         <v>236</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4109,7 +4183,7 @@
         <v>293</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4126,7 +4200,7 @@
         <v>374</v>
       </c>
       <c r="E38" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4143,7 +4217,7 @@
         <v>374</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4160,7 +4234,7 @@
         <v>457</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4177,7 +4251,7 @@
         <v>552</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4194,7 +4268,7 @@
         <v>683</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4211,12 +4285,12 @@
         <v>683</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>4</v>
@@ -4228,7 +4302,7 @@
         <v>683</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4245,12 +4319,12 @@
         <v>683</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>4</v>
@@ -4262,12 +4336,12 @@
         <v>102</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>4</v>
@@ -4279,12 +4353,12 @@
         <v>273</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>4</v>
@@ -4296,12 +4370,12 @@
         <v>273</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>4</v>
@@ -4313,12 +4387,12 @@
         <v>442</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>4</v>
@@ -4330,12 +4404,12 @@
         <v>442</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>4</v>
@@ -4347,12 +4421,12 @@
         <v>388</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>4</v>
@@ -4364,12 +4438,12 @@
         <v>388</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>4</v>
@@ -4381,12 +4455,12 @@
         <v>388</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>4</v>
@@ -4398,12 +4472,12 @@
         <v>70</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>4</v>
@@ -4415,12 +4489,12 @@
         <v>134</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>4</v>
@@ -4432,12 +4506,12 @@
         <v>32</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>4</v>
@@ -4449,7 +4523,7 @@
         <v>32</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -4474,15 +4548,15 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B4">
         <v>18</v>
@@ -4490,7 +4564,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -4498,7 +4572,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B6">
         <v>28</v>
@@ -4506,7 +4580,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B7">
         <v>13</v>

</xml_diff>